<commit_message>
Deleted wrong info in sensors
</commit_message>
<xml_diff>
--- a/docs/DOC-Files/DOC-001-Bill_Of_Materials.xlsx
+++ b/docs/DOC-Files/DOC-001-Bill_Of_Materials.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camillabjelven/Documents/GitHub/SLaRC-LightSeeker-HT25/docs/DOC-Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81E80479-7767-BA4C-B326-6D022EE8B26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C632C0B-6925-494F-93AA-CC4A0F39CBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="170">
   <si>
     <t>Bill Of Materials</t>
   </si>
@@ -541,7 +541,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,12 +637,6 @@
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -689,9 +683,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -718,9 +709,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1032,10 +1032,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1045,16 +1047,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="49" x14ac:dyDescent="0.55000000000000004">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="6" spans="2:10" ht="30" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
@@ -1071,39 +1073,39 @@
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.35">
@@ -1149,20 +1151,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="10" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="13" customWidth="1"/>
+    <col min="7" max="7" width="14" style="11" customWidth="1"/>
     <col min="8" max="10" width="8.83203125" customWidth="1"/>
     <col min="11" max="11" width="29.1640625" customWidth="1"/>
     <col min="12" max="12" width="21.6640625" customWidth="1"/>
@@ -1171,61 +1173,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1237,25 +1239,25 @@
       <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>865060757007</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H3">
         <v>3</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="13" t="s">
         <v>25</v>
       </c>
       <c r="M3" t="s">
@@ -1272,25 +1274,25 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="11">
         <v>885012208087</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="13" t="s">
         <v>30</v>
       </c>
       <c r="M4" t="s">
@@ -1307,25 +1309,25 @@
       <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="11">
         <v>865080643008</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="13" t="s">
         <v>35</v>
       </c>
       <c r="M5" t="s">
@@ -1342,25 +1344,25 @@
       <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="11">
         <v>6917399</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="13" t="s">
         <v>43</v>
       </c>
       <c r="M6" t="s">
@@ -1377,25 +1379,25 @@
       <c r="C7" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>47</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="13" t="s">
         <v>43</v>
       </c>
       <c r="M7" t="s">
@@ -1412,25 +1414,25 @@
       <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>54</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="11">
         <v>6882003</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="13" t="s">
         <v>56</v>
       </c>
       <c r="M8" t="s">
@@ -1447,25 +1449,25 @@
       <c r="C9" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>61</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="11">
         <v>8949600</v>
       </c>
       <c r="H9">
         <v>11</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="13" t="s">
         <v>63</v>
       </c>
       <c r="M9" t="s">
@@ -1482,12 +1484,12 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="E10" s="11"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1499,12 +1501,12 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="E11" s="11"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1516,12 +1518,12 @@
       <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
+      <c r="E12" s="11"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1533,25 +1535,25 @@
       <c r="C13" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="10" t="s">
         <v>69</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H13">
         <v>3</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="13" t="s">
         <v>72</v>
       </c>
       <c r="M13" t="s">
@@ -1568,25 +1570,25 @@
       <c r="C14" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="10" t="s">
         <v>77</v>
       </c>
       <c r="F14" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="11">
         <v>41020964</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="13" t="s">
         <v>80</v>
       </c>
       <c r="M14" t="s">
@@ -1603,25 +1605,25 @@
       <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>83</v>
       </c>
       <c r="F15" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="11">
         <v>41023790</v>
       </c>
       <c r="H15">
         <v>11</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="13" t="s">
         <v>85</v>
       </c>
       <c r="M15" t="s">
@@ -1629,20 +1631,20 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
     </row>
     <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -1654,25 +1656,25 @@
       <c r="C18" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="10" t="s">
         <v>77</v>
       </c>
       <c r="F18" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="11">
         <v>41020964</v>
       </c>
       <c r="H18">
         <v>2</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="13" t="s">
         <v>80</v>
       </c>
       <c r="M18" t="s">
@@ -1689,25 +1691,25 @@
       <c r="C19" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="10" t="s">
         <v>90</v>
       </c>
       <c r="F19" t="s">
         <v>78</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="11">
         <v>41023547</v>
       </c>
       <c r="H19">
         <v>4</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="13" t="s">
         <v>92</v>
       </c>
       <c r="M19" t="s">
@@ -1724,25 +1726,25 @@
       <c r="C20" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="10" t="s">
         <v>83</v>
       </c>
       <c r="F20" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="11">
         <v>41023790</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L20" s="13" t="s">
         <v>85</v>
       </c>
       <c r="M20" t="s">
@@ -1762,16 +1764,16 @@
       <c r="F21" t="s">
         <v>78</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="11">
         <v>41018322</v>
       </c>
       <c r="H21">
         <v>4</v>
       </c>
-      <c r="K21" s="15" t="s">
+      <c r="K21" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="L21" s="15" t="s">
+      <c r="L21" s="13" t="s">
         <v>98</v>
       </c>
       <c r="M21" t="s">
@@ -1788,25 +1790,25 @@
       <c r="C22" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="11" t="s">
         <v>61</v>
       </c>
       <c r="F22" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="11">
         <v>8949600</v>
       </c>
       <c r="H22">
         <v>5</v>
       </c>
-      <c r="K22" s="15" t="s">
+      <c r="K22" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L22" s="15" t="s">
+      <c r="L22" s="13" t="s">
         <v>63</v>
       </c>
       <c r="M22" t="s">
@@ -1842,22 +1844,22 @@
       <c r="B25" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>102</v>
       </c>
       <c r="F25" t="s">
         <v>103</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="11" t="s">
         <v>104</v>
       </c>
       <c r="H25">
         <v>2</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="L25" s="15" t="s">
+      <c r="L25" s="13" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1868,15 +1870,15 @@
       <c r="B26" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="10"/>
       <c r="F26" t="s">
         <v>108</v>
       </c>
       <c r="H26">
         <v>3</v>
       </c>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -1890,14 +1892,14 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C30" s="12"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
+      <c r="C30" s="10"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C31" s="12"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
+      <c r="C31" s="10"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1905,45 +1907,45 @@
     <mergeCell ref="A17:C17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" location="865060757007"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="K4" r:id="rId3" location="885012208087"/>
-    <hyperlink ref="L4" r:id="rId4"/>
-    <hyperlink ref="K5" r:id="rId5" location="865080643008"/>
-    <hyperlink ref="L5" r:id="rId6"/>
-    <hyperlink ref="K6" r:id="rId7"/>
-    <hyperlink ref="L6" r:id="rId8"/>
-    <hyperlink ref="K7" r:id="rId9"/>
-    <hyperlink ref="L7" r:id="rId10"/>
-    <hyperlink ref="K8" r:id="rId11"/>
-    <hyperlink ref="L8" r:id="rId12"/>
-    <hyperlink ref="K9" r:id="rId13"/>
-    <hyperlink ref="L9" r:id="rId14"/>
-    <hyperlink ref="K13" r:id="rId15"/>
-    <hyperlink ref="L13" r:id="rId16"/>
-    <hyperlink ref="K14" r:id="rId17"/>
-    <hyperlink ref="L14" r:id="rId18"/>
-    <hyperlink ref="K15" r:id="rId19"/>
-    <hyperlink ref="L15" r:id="rId20"/>
-    <hyperlink ref="K18" r:id="rId21"/>
-    <hyperlink ref="L18" r:id="rId22"/>
-    <hyperlink ref="K19" r:id="rId23"/>
-    <hyperlink ref="L19" r:id="rId24"/>
-    <hyperlink ref="K20" r:id="rId25"/>
-    <hyperlink ref="L20" r:id="rId26"/>
-    <hyperlink ref="K21" r:id="rId27"/>
-    <hyperlink ref="L21" r:id="rId28"/>
-    <hyperlink ref="K22" r:id="rId29"/>
-    <hyperlink ref="L22" r:id="rId30"/>
-    <hyperlink ref="K25" r:id="rId31"/>
-    <hyperlink ref="L25" r:id="rId32"/>
+    <hyperlink ref="K3" r:id="rId1" location="865060757007" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="K4" r:id="rId3" location="885012208087" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="L4" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="K5" r:id="rId5" location="865080643008" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="L5" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="K6" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="L6" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="K7" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="L7" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="K8" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="L8" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="K9" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="L9" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="K13" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="L13" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="K14" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="L14" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="K15" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="L15" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="K18" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="L18" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="K19" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="L19" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="K20" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="L20" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="K21" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="L21" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="K22" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="L22" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="K25" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="L25" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1953,10 +1955,10 @@
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="10" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="13" customWidth="1"/>
+    <col min="7" max="7" width="14" style="11" customWidth="1"/>
     <col min="8" max="9" width="8.83203125" customWidth="1"/>
     <col min="10" max="10" width="29.5" customWidth="1"/>
     <col min="11" max="11" width="29.1640625" customWidth="1"/>
@@ -1966,58 +1968,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
       <c r="G2"/>
-      <c r="I2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -2026,10 +2028,10 @@
       <c r="B3" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F3" t="s">
@@ -2042,10 +2044,10 @@
       <c r="J3" t="s">
         <v>115</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2056,13 +2058,13 @@
       <c r="B4" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F4" t="s">
@@ -2072,10 +2074,10 @@
       <c r="H4">
         <v>8</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2086,13 +2088,13 @@
       <c r="B5" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="11"/>
       <c r="F5" t="s">
         <v>114</v>
       </c>
@@ -2103,10 +2105,10 @@
       <c r="J5" t="s">
         <v>120</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2117,13 +2119,13 @@
       <c r="B6" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="18" t="s">
         <v>23</v>
       </c>
       <c r="F6" t="s">
@@ -2136,10 +2138,10 @@
       <c r="J6" t="s">
         <v>122</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2150,10 +2152,10 @@
       <c r="B7" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="18" t="s">
         <v>23</v>
       </c>
       <c r="F7" t="s">
@@ -2166,10 +2168,10 @@
       <c r="J7" t="s">
         <v>125</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2180,20 +2182,20 @@
       <c r="B8" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="18" t="s">
         <v>23</v>
       </c>
       <c r="F8" t="s">
         <v>114</v>
       </c>
       <c r="G8"/>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2216,10 +2218,10 @@
       <c r="J9" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="13" t="s">
         <v>134</v>
       </c>
       <c r="M9" t="s">
@@ -2233,7 +2235,7 @@
       <c r="B10" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="11"/>
       <c r="F10" t="s">
         <v>130</v>
       </c>
@@ -2244,10 +2246,10 @@
       <c r="J10" t="s">
         <v>137</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="13" t="s">
         <v>139</v>
       </c>
       <c r="M10" t="s">
@@ -2261,7 +2263,7 @@
       <c r="B11" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="11"/>
       <c r="F11" t="s">
         <v>142</v>
       </c>
@@ -2269,8 +2271,8 @@
       <c r="H11">
         <v>4</v>
       </c>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -2282,16 +2284,16 @@
       <c r="F12" t="s">
         <v>144</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="11">
         <v>10818</v>
       </c>
       <c r="H12">
         <v>4</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2305,37 +2307,37 @@
       <c r="F13" t="s">
         <v>144</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="11" t="s">
         <v>147</v>
       </c>
       <c r="H13">
         <v>4</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K15" s="15"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
     </row>
     <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -2344,20 +2346,20 @@
       <c r="B18" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="10"/>
       <c r="F18" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="11" t="s">
         <v>152</v>
       </c>
       <c r="H18">
         <v>2</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2368,20 +2370,20 @@
       <c r="B19" t="s">
         <v>154</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="10"/>
       <c r="F19" t="s">
         <v>151</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>155</v>
       </c>
       <c r="H19">
         <v>2</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2392,7 +2394,7 @@
       <c r="B20" t="s">
         <v>157</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>158</v>
       </c>
       <c r="F20" t="s">
@@ -2401,8 +2403,8 @@
       <c r="H20">
         <v>3</v>
       </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -2411,12 +2413,12 @@
       <c r="B21" t="s">
         <v>159</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
+      <c r="E21" s="11"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -2429,39 +2431,41 @@
     <mergeCell ref="A17:C17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1"/>
-    <hyperlink ref="K4" r:id="rId2"/>
-    <hyperlink ref="K5" r:id="rId3"/>
-    <hyperlink ref="K6" r:id="rId4"/>
-    <hyperlink ref="K7" r:id="rId5"/>
-    <hyperlink ref="K8" r:id="rId6"/>
-    <hyperlink ref="K9" r:id="rId7"/>
-    <hyperlink ref="L9" r:id="rId8"/>
-    <hyperlink ref="K10" r:id="rId9"/>
-    <hyperlink ref="L10" r:id="rId10"/>
-    <hyperlink ref="K12" r:id="rId11" location="/11-farg-svart"/>
-    <hyperlink ref="K18" r:id="rId12"/>
-    <hyperlink ref="K19" r:id="rId13"/>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="K5" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="K6" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="K7" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="K8" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="K9" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="L9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="K10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="L10" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="K12" r:id="rId11" location="/11-farg-svart" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="K18" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="K19" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="10" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="13" customWidth="1"/>
+    <col min="7" max="7" width="14" style="11" customWidth="1"/>
     <col min="8" max="10" width="8.83203125" customWidth="1"/>
     <col min="11" max="11" width="29.1640625" customWidth="1"/>
     <col min="12" max="12" width="21.6640625" customWidth="1"/>
@@ -2470,214 +2474,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="E9" s="11"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="E10" s="11"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="E11" s="11"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
+      <c r="E12" s="11"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
+      <c r="E22" s="11"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -2714,20 +2714,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="10" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="13" customWidth="1"/>
+    <col min="7" max="7" width="14" style="11" customWidth="1"/>
     <col min="8" max="9" width="8.83203125" customWidth="1"/>
     <col min="10" max="10" width="29.5" customWidth="1"/>
     <col min="11" max="11" width="29.1640625" customWidth="1"/>
@@ -2737,94 +2739,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
       <c r="G2"/>
-      <c r="I2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
       <c r="G4"/>
-      <c r="I4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="I4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -2833,10 +2835,10 @@
       <c r="B5" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F5" t="s">
@@ -2846,10 +2848,10 @@
       <c r="J5" t="s">
         <v>115</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="L5" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2860,23 +2862,23 @@
       <c r="B6" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F6" t="s">
         <v>114</v>
       </c>
       <c r="G6"/>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2887,13 +2889,13 @@
       <c r="B7" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="11"/>
       <c r="F7" t="s">
         <v>114</v>
       </c>
@@ -2901,10 +2903,10 @@
       <c r="J7" t="s">
         <v>120</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="L7" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2915,13 +2917,13 @@
       <c r="B8" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F8" t="s">
@@ -2931,10 +2933,10 @@
       <c r="J8" t="s">
         <v>122</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="L8" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2945,10 +2947,10 @@
       <c r="B9" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F9" t="s">
@@ -2958,10 +2960,10 @@
       <c r="J9" t="s">
         <v>125</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="L9" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2972,20 +2974,20 @@
       <c r="B10" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F10" t="s">
         <v>114</v>
       </c>
       <c r="G10"/>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="L10" s="26" t="s">
+      <c r="L10" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3008,10 +3010,10 @@
       <c r="J11" t="s">
         <v>132</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="13" t="s">
         <v>134</v>
       </c>
       <c r="M11" t="s">
@@ -3025,7 +3027,7 @@
       <c r="B12" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="11"/>
       <c r="F12" t="s">
         <v>130</v>
       </c>
@@ -3036,10 +3038,10 @@
       <c r="J12" t="s">
         <v>137</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="13" t="s">
         <v>139</v>
       </c>
       <c r="M12" t="s">
@@ -3053,7 +3055,7 @@
       <c r="B13" t="s">
         <v>141</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="11"/>
       <c r="F13" t="s">
         <v>142</v>
       </c>
@@ -3061,8 +3063,8 @@
       <c r="H13" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -3074,16 +3076,16 @@
       <c r="F14" t="s">
         <v>144</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="11">
         <v>10818</v>
       </c>
       <c r="H14" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3097,37 +3099,37 @@
       <c r="F15" t="s">
         <v>144</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="11" t="s">
         <v>147</v>
       </c>
       <c r="H15" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="K16" s="15"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
     </row>
     <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -3136,20 +3138,20 @@
       <c r="B18" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="10"/>
       <c r="F18" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="11" t="s">
         <v>152</v>
       </c>
       <c r="H18">
         <v>2</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3160,20 +3162,20 @@
       <c r="B19" t="s">
         <v>154</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="10"/>
       <c r="F19" t="s">
         <v>151</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>155</v>
       </c>
       <c r="H19">
         <v>2</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3184,7 +3186,7 @@
       <c r="B20" t="s">
         <v>157</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>158</v>
       </c>
       <c r="F20" t="s">
@@ -3193,55 +3195,55 @@
       <c r="H20">
         <v>3</v>
       </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
+      <c r="C21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C22" s="12"/>
-      <c r="E22" s="13"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
+      <c r="C22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C23" s="12"/>
-      <c r="E23" s="13"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
+      <c r="C23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-    </row>
-    <row r="25" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
+      <c r="C24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="27"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
     </row>
     <row r="26" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
@@ -3250,25 +3252,25 @@
       <c r="C26" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="11">
         <v>865060757007</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="13" t="s">
+      <c r="F26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H26">
         <v>3</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="K26" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="15" t="s">
+      <c r="L26" s="13" t="s">
         <v>25</v>
       </c>
       <c r="M26" t="s">
@@ -3282,25 +3284,25 @@
       <c r="C27" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="11">
         <v>885012208087</v>
       </c>
-      <c r="F27" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="13" t="s">
+      <c r="F27" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H27">
         <v>3</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K27" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L27" s="15" t="s">
+      <c r="L27" s="13" t="s">
         <v>30</v>
       </c>
       <c r="M27" t="s">
@@ -3314,25 +3316,25 @@
       <c r="C28" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="11">
         <v>865080643008</v>
       </c>
-      <c r="F28" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="13" t="s">
+      <c r="F28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H28">
         <v>3</v>
       </c>
-      <c r="K28" s="15" t="s">
+      <c r="K28" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="L28" s="13" t="s">
         <v>35</v>
       </c>
       <c r="M28" t="s">
@@ -3346,25 +3348,25 @@
       <c r="C29" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F29" t="s">
         <v>41</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="11">
         <v>6917399</v>
       </c>
       <c r="H29">
         <v>2</v>
       </c>
-      <c r="K29" s="15" t="s">
+      <c r="K29" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="L29" s="13" t="s">
         <v>43</v>
       </c>
       <c r="M29" t="s">
@@ -3378,25 +3380,25 @@
       <c r="C30" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="10" t="s">
         <v>47</v>
       </c>
       <c r="F30" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="11" t="s">
         <v>48</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
-      <c r="K30" s="15" t="s">
+      <c r="K30" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="13" t="s">
         <v>43</v>
       </c>
       <c r="M30" t="s">
@@ -3410,25 +3412,25 @@
       <c r="C31" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="10" t="s">
         <v>54</v>
       </c>
       <c r="F31" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="11">
         <v>6882003</v>
       </c>
       <c r="H31">
         <v>3</v>
       </c>
-      <c r="K31" s="15" t="s">
+      <c r="K31" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="13" t="s">
         <v>56</v>
       </c>
       <c r="M31" t="s">
@@ -3442,25 +3444,25 @@
       <c r="C32" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="11" t="s">
         <v>61</v>
       </c>
       <c r="F32" t="s">
         <v>41</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="11">
         <v>8949600</v>
       </c>
       <c r="H32">
         <v>11</v>
       </c>
-      <c r="K32" s="15" t="s">
+      <c r="K32" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L32" s="15" t="s">
+      <c r="L32" s="13" t="s">
         <v>63</v>
       </c>
       <c r="M32" t="s">
@@ -3474,12 +3476,12 @@
       <c r="C33" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
+      <c r="E33" s="11"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
@@ -3488,12 +3490,12 @@
       <c r="C34" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
+      <c r="E34" s="11"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
@@ -3502,12 +3504,12 @@
       <c r="C35" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="13"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
+      <c r="E35" s="11"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
@@ -3516,25 +3518,25 @@
       <c r="C36" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="10" t="s">
         <v>69</v>
       </c>
       <c r="F36" t="s">
         <v>41</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H36">
         <v>3</v>
       </c>
-      <c r="K36" s="15" t="s">
+      <c r="K36" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="L36" s="15" t="s">
+      <c r="L36" s="13" t="s">
         <v>72</v>
       </c>
       <c r="M36" t="s">
@@ -3548,25 +3550,25 @@
       <c r="C37" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="10" t="s">
         <v>77</v>
       </c>
       <c r="F37" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="11">
         <v>41020964</v>
       </c>
       <c r="H37">
         <v>1</v>
       </c>
-      <c r="K37" s="15" t="s">
+      <c r="K37" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="L37" s="15" t="s">
+      <c r="L37" s="13" t="s">
         <v>80</v>
       </c>
       <c r="M37" t="s">
@@ -3580,53 +3582,53 @@
       <c r="C38" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="10" t="s">
         <v>83</v>
       </c>
       <c r="F38" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G38" s="11">
         <v>41023790</v>
       </c>
       <c r="H38">
         <v>11</v>
       </c>
-      <c r="K38" s="15" t="s">
+      <c r="K38" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="L38" s="15" t="s">
+      <c r="L38" s="13" t="s">
         <v>85</v>
       </c>
       <c r="M38" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="27" t="s">
+    <row r="41" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="24"/>
     </row>
     <row r="42" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
@@ -3635,25 +3637,25 @@
       <c r="C42" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="10" t="s">
         <v>77</v>
       </c>
       <c r="F42" t="s">
         <v>78</v>
       </c>
-      <c r="G42" s="13">
+      <c r="G42" s="11">
         <v>41020964</v>
       </c>
       <c r="H42">
         <v>2</v>
       </c>
-      <c r="K42" s="15" t="s">
+      <c r="K42" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="L42" s="15" t="s">
+      <c r="L42" s="13" t="s">
         <v>80</v>
       </c>
       <c r="M42" t="s">
@@ -3667,25 +3669,25 @@
       <c r="C43" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="10" t="s">
         <v>90</v>
       </c>
       <c r="F43" t="s">
         <v>78</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="11">
         <v>41023547</v>
       </c>
       <c r="H43">
         <v>4</v>
       </c>
-      <c r="K43" s="15" t="s">
+      <c r="K43" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="L43" s="15" t="s">
+      <c r="L43" s="13" t="s">
         <v>92</v>
       </c>
       <c r="M43" t="s">
@@ -3699,25 +3701,25 @@
       <c r="C44" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="10" t="s">
         <v>83</v>
       </c>
       <c r="F44" t="s">
         <v>78</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="11">
         <v>41023790</v>
       </c>
       <c r="H44">
         <v>2</v>
       </c>
-      <c r="K44" s="15" t="s">
+      <c r="K44" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="L44" s="15" t="s">
+      <c r="L44" s="13" t="s">
         <v>85</v>
       </c>
       <c r="M44" t="s">
@@ -3734,16 +3736,16 @@
       <c r="F45" t="s">
         <v>78</v>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="11">
         <v>41018322</v>
       </c>
       <c r="H45">
         <v>4</v>
       </c>
-      <c r="K45" s="15" t="s">
+      <c r="K45" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="L45" s="15" t="s">
+      <c r="L45" s="13" t="s">
         <v>98</v>
       </c>
       <c r="M45" t="s">
@@ -3757,25 +3759,25 @@
       <c r="C46" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E46" s="11" t="s">
         <v>61</v>
       </c>
       <c r="F46" t="s">
         <v>41</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="11">
         <v>8949600</v>
       </c>
       <c r="H46">
         <v>5</v>
       </c>
-      <c r="K46" s="15" t="s">
+      <c r="K46" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L46" s="15" t="s">
+      <c r="L46" s="13" t="s">
         <v>63</v>
       </c>
       <c r="M46" t="s">
@@ -3823,20 +3825,20 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A79" s="20" t="s">
+      <c r="A79" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="16"/>
-      <c r="E79" s="16"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="18"/>
-      <c r="H79" s="19"/>
-      <c r="I79" s="19"/>
-      <c r="J79" s="19"/>
-      <c r="K79" s="19"/>
-      <c r="L79" s="19"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+      <c r="J79" s="17"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="17"/>
     </row>
     <row r="80" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -3845,11 +3847,11 @@
       <c r="B80" t="s">
         <v>166</v>
       </c>
-      <c r="C80" s="12"/>
+      <c r="C80" s="10"/>
       <c r="F80" t="s">
         <v>151</v>
       </c>
-      <c r="G80" s="13" t="s">
+      <c r="G80" s="11" t="s">
         <v>167</v>
       </c>
       <c r="H80">
@@ -3858,10 +3860,10 @@
       <c r="J80" t="s">
         <v>168</v>
       </c>
-      <c r="K80" s="32" t="s">
+      <c r="K80" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="L80" s="15"/>
+      <c r="L80" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3871,49 +3873,49 @@
     <mergeCell ref="A79:C79"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K5" r:id="rId1"/>
-    <hyperlink ref="K6" r:id="rId2"/>
-    <hyperlink ref="K7" r:id="rId3"/>
-    <hyperlink ref="K8" r:id="rId4"/>
-    <hyperlink ref="K9" r:id="rId5"/>
-    <hyperlink ref="K10" r:id="rId6"/>
-    <hyperlink ref="K11" r:id="rId7"/>
-    <hyperlink ref="L11" r:id="rId8"/>
-    <hyperlink ref="K12" r:id="rId9"/>
-    <hyperlink ref="L12" r:id="rId10"/>
-    <hyperlink ref="K14" r:id="rId11" location="/11-farg-svart"/>
-    <hyperlink ref="K18" r:id="rId12"/>
-    <hyperlink ref="K19" r:id="rId13"/>
-    <hyperlink ref="K26" r:id="rId14" location="865060757007"/>
-    <hyperlink ref="L26" r:id="rId15"/>
-    <hyperlink ref="K27" r:id="rId16" location="885012208087"/>
-    <hyperlink ref="L27" r:id="rId17"/>
-    <hyperlink ref="K28" r:id="rId18" location="865080643008"/>
-    <hyperlink ref="L28" r:id="rId19"/>
-    <hyperlink ref="K29" r:id="rId20"/>
-    <hyperlink ref="L29" r:id="rId21"/>
-    <hyperlink ref="K30" r:id="rId22"/>
-    <hyperlink ref="L30" r:id="rId23"/>
-    <hyperlink ref="K31" r:id="rId24"/>
-    <hyperlink ref="L31" r:id="rId25"/>
-    <hyperlink ref="K32" r:id="rId26"/>
-    <hyperlink ref="L32" r:id="rId27"/>
-    <hyperlink ref="K36" r:id="rId28"/>
-    <hyperlink ref="L36" r:id="rId29"/>
-    <hyperlink ref="K37" r:id="rId30"/>
-    <hyperlink ref="L37" r:id="rId31"/>
-    <hyperlink ref="K38" r:id="rId32"/>
-    <hyperlink ref="L38" r:id="rId33"/>
-    <hyperlink ref="K42" r:id="rId34"/>
-    <hyperlink ref="L42" r:id="rId35"/>
-    <hyperlink ref="K43" r:id="rId36"/>
-    <hyperlink ref="L43" r:id="rId37"/>
-    <hyperlink ref="K44" r:id="rId38"/>
-    <hyperlink ref="L44" r:id="rId39"/>
-    <hyperlink ref="K45" r:id="rId40"/>
-    <hyperlink ref="L45" r:id="rId41"/>
-    <hyperlink ref="K46" r:id="rId42"/>
-    <hyperlink ref="L46" r:id="rId43"/>
+    <hyperlink ref="K5" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="K6" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="K7" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="K8" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="K9" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="K10" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="K11" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="L11" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="K12" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="L12" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="K14" r:id="rId11" location="/11-farg-svart" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="K18" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="K19" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="K26" r:id="rId14" location="865060757007" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="L26" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="K27" r:id="rId16" location="885012208087" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="L27" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="K28" r:id="rId18" location="865080643008" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="L28" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="K29" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="L29" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="K30" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="L30" r:id="rId23" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="K31" r:id="rId24" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="L31" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="K32" r:id="rId26" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
+    <hyperlink ref="L32" r:id="rId27" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
+    <hyperlink ref="K36" r:id="rId28" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
+    <hyperlink ref="L36" r:id="rId29" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
+    <hyperlink ref="K37" r:id="rId30" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
+    <hyperlink ref="L37" r:id="rId31" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
+    <hyperlink ref="K38" r:id="rId32" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
+    <hyperlink ref="L38" r:id="rId33" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
+    <hyperlink ref="K42" r:id="rId34" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
+    <hyperlink ref="L42" r:id="rId35" xr:uid="{00000000-0004-0000-0400-000022000000}"/>
+    <hyperlink ref="K43" r:id="rId36" xr:uid="{00000000-0004-0000-0400-000023000000}"/>
+    <hyperlink ref="L43" r:id="rId37" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
+    <hyperlink ref="K44" r:id="rId38" xr:uid="{00000000-0004-0000-0400-000025000000}"/>
+    <hyperlink ref="L44" r:id="rId39" xr:uid="{00000000-0004-0000-0400-000026000000}"/>
+    <hyperlink ref="K45" r:id="rId40" xr:uid="{00000000-0004-0000-0400-000027000000}"/>
+    <hyperlink ref="L45" r:id="rId41" xr:uid="{00000000-0004-0000-0400-000028000000}"/>
+    <hyperlink ref="K46" r:id="rId42" xr:uid="{00000000-0004-0000-0400-000029000000}"/>
+    <hyperlink ref="L46" r:id="rId43" xr:uid="{00000000-0004-0000-0400-00002A000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>

</xml_diff>